<commit_message>
Deploying to gh-pages from  @ c5bd2913746a367c570d362c9cc856e958e8d611 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/5.2.1.1b.xlsx
+++ b/en/downloads/data-excel/5.2.1.1b.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>5.2.1.1b Жынысы, курактык топтор, билим деңгээли жана иши боюнча үй-бүлөлүк зомбулуктан жабыр тарткандардын саны</t>
   </si>
@@ -52,42 +52,6 @@
     <t>Kyrgyz Republic</t>
   </si>
   <si>
-    <t>жынысы боюнча:</t>
-  </si>
-  <si>
-    <t>по полу:</t>
-  </si>
-  <si>
-    <t>by sex:</t>
-  </si>
-  <si>
-    <t>аялдар</t>
-  </si>
-  <si>
-    <t>женщины</t>
-  </si>
-  <si>
-    <t>women</t>
-  </si>
-  <si>
-    <t>эркектер</t>
-  </si>
-  <si>
-    <t>мужчины</t>
-  </si>
-  <si>
-    <t>men</t>
-  </si>
-  <si>
-    <t>курак топтор боюнча, жаш:</t>
-  </si>
-  <si>
-    <t>по возрастным группам, лет:</t>
-  </si>
-  <si>
-    <t>by age group, years:</t>
-  </si>
-  <si>
     <t xml:space="preserve">        20га чейин</t>
   </si>
   <si>
@@ -124,103 +88,142 @@
     <t>        51 and older</t>
   </si>
   <si>
-    <t>билим деңгээли боюнча:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> по уровню образования:</t>
-  </si>
-  <si>
-    <t>by level of education:</t>
-  </si>
-  <si>
-    <t>жогорку кесиптик</t>
-  </si>
-  <si>
-    <t>высшее профессиональное</t>
-  </si>
-  <si>
-    <t>higher professional</t>
-  </si>
-  <si>
-    <t>бүтпөгөн жогорку кесиптик</t>
-  </si>
-  <si>
-    <t>незаконченное высшее профессиональное</t>
-  </si>
-  <si>
-    <t>incomplete higher professional</t>
-  </si>
-  <si>
-    <t>орто кесиптик</t>
-  </si>
-  <si>
-    <t>среднее профессиональное</t>
-  </si>
-  <si>
-    <t>secondary vocational</t>
-  </si>
-  <si>
-    <t>жалпы орто</t>
-  </si>
-  <si>
-    <t>среднее общее</t>
-  </si>
-  <si>
-    <t>average total</t>
-  </si>
-  <si>
-    <t>башка</t>
-  </si>
-  <si>
-    <t>другое</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>иши боюнча:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> по роду занятий:</t>
-  </si>
-  <si>
-    <t> by occupation:</t>
-  </si>
-  <si>
-    <t>иштешет</t>
-  </si>
-  <si>
-    <t xml:space="preserve">работают </t>
-  </si>
-  <si>
-    <t>are working</t>
-  </si>
-  <si>
-    <t>иштешпейт</t>
-  </si>
-  <si>
-    <t>не работают</t>
-  </si>
-  <si>
-    <t>does not work</t>
-  </si>
-  <si>
-    <t>окушат, студенттер</t>
-  </si>
-  <si>
-    <t>учащиеся, студенты</t>
-  </si>
-  <si>
-    <t>pupils, students</t>
-  </si>
-  <si>
-    <t>пенсионерлер</t>
-  </si>
-  <si>
-    <t>пенсионеры</t>
-  </si>
-  <si>
-    <t>seniors</t>
+    <t>…</t>
+  </si>
+  <si>
+    <t>By sex:</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>By level of education:</t>
+  </si>
+  <si>
+    <t>Higher professional</t>
+  </si>
+  <si>
+    <t>Incomplete higher professional</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t> By occupation:</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>Pensioners</t>
+  </si>
+  <si>
+    <t>Secondary professional</t>
+  </si>
+  <si>
+    <t>Secondary general</t>
+  </si>
+  <si>
+    <t>По полу:</t>
+  </si>
+  <si>
+    <t>Жынысы боюнча:</t>
+  </si>
+  <si>
+    <t>Аялдар</t>
+  </si>
+  <si>
+    <t>Эркектер</t>
+  </si>
+  <si>
+    <t>Женщины</t>
+  </si>
+  <si>
+    <t>Мужчины</t>
+  </si>
+  <si>
+    <t>Билим деңгээли боюнча:</t>
+  </si>
+  <si>
+    <t>Жогорку кесиптик</t>
+  </si>
+  <si>
+    <t>Бүтпөгөн жогорку кесиптик</t>
+  </si>
+  <si>
+    <t>Орто кесиптик</t>
+  </si>
+  <si>
+    <t>Жалпы орто</t>
+  </si>
+  <si>
+    <t>Башка</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> По уровню образования:</t>
+  </si>
+  <si>
+    <t>По возрастным группам, лет:</t>
+  </si>
+  <si>
+    <t>Жаш курак топтор боюнча, жаш:</t>
+  </si>
+  <si>
+    <t>By age group, years:</t>
+  </si>
+  <si>
+    <t>Высшее профессиональное</t>
+  </si>
+  <si>
+    <t>Незаконченное высшее профессиональное</t>
+  </si>
+  <si>
+    <t>Среднее профессиональное</t>
+  </si>
+  <si>
+    <t>Среднее общее</t>
+  </si>
+  <si>
+    <t>Другое</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> По роду занятий:</t>
+  </si>
+  <si>
+    <t>Иши боюнча:</t>
+  </si>
+  <si>
+    <t>Иштешет</t>
+  </si>
+  <si>
+    <t>Иштешпейт</t>
+  </si>
+  <si>
+    <t>Окушат, студенттер</t>
+  </si>
+  <si>
+    <t>Пенсионерлер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Работают </t>
+  </si>
+  <si>
+    <t>Не работают</t>
+  </si>
+  <si>
+    <t>Учащиеся, студенты</t>
+  </si>
+  <si>
+    <t>Пенсионеры</t>
   </si>
 </sst>
 </file>
@@ -267,13 +270,14 @@
       <charset val="204"/>
     </font>
     <font>
-      <i/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -309,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -341,19 +345,29 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -730,7 +744,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="3"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -775,7 +789,9 @@
       <c r="N4" s="8">
         <v>2019</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="O4" s="15">
+        <v>2020</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -820,17 +836,19 @@
       <c r="N5" s="9">
         <v>6145</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="16">
+        <v>8254</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>14</v>
+      <c r="A6" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -843,107 +861,111 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="O6" s="17"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="12">
+        <v>26</v>
+      </c>
+      <c r="D7" s="11">
         <v>1927</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>1659</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>1714</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>2341</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>2269</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>2531</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <v>3229</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <v>6795</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>6966</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <v>6562</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="12">
         <v>5659</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="O7" s="16">
+        <v>7891</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="12">
+        <v>27</v>
+      </c>
+      <c r="D8" s="11">
         <v>166</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>130</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>95</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>74</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>70</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>98</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <v>104</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <v>210</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="12">
         <v>357</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <v>616</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="12">
         <v>486</v>
       </c>
-      <c r="O8" s="3"/>
+      <c r="O8" s="18">
+        <v>363</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
+      <c r="A9" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -956,34 +978,34 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="O9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="14">
+        <v>14</v>
+      </c>
+      <c r="D10" s="13">
         <v>126</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>212</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>37</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>92</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>73</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <v>100</v>
       </c>
       <c r="J10" s="3">
@@ -1001,34 +1023,36 @@
       <c r="N10" s="3">
         <v>561</v>
       </c>
-      <c r="O10" s="3"/>
+      <c r="O10" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="14">
+        <v>16</v>
+      </c>
+      <c r="D11" s="13">
         <v>738</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>634</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>476</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>654</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>678</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <v>837</v>
       </c>
       <c r="J11" s="3">
@@ -1037,43 +1061,45 @@
       <c r="K11" s="3">
         <v>2085</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="13">
         <v>1888</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="13">
         <v>2108</v>
       </c>
       <c r="N11" s="3">
         <v>1879</v>
       </c>
-      <c r="O11" s="3"/>
+      <c r="O11" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="14">
+        <v>18</v>
+      </c>
+      <c r="D12" s="13">
         <v>762</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>552</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>687</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>1108</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>957</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="13">
         <v>904</v>
       </c>
       <c r="J12" s="3">
@@ -1082,43 +1108,45 @@
       <c r="K12" s="3">
         <v>2422</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="13">
         <v>2531</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="13">
         <v>2385</v>
       </c>
       <c r="N12" s="3">
         <v>1974</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="O12" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="14">
+        <v>20</v>
+      </c>
+      <c r="D13" s="13">
         <v>336</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <v>283</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="13">
         <v>461</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>424</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <v>463</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="13">
         <v>482</v>
       </c>
       <c r="J13" s="3">
@@ -1127,43 +1155,45 @@
       <c r="K13" s="3">
         <v>1435</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="13">
         <v>1496</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="13">
         <v>1550</v>
       </c>
       <c r="N13" s="3">
         <v>1121</v>
       </c>
-      <c r="O13" s="3"/>
+      <c r="O13" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="14">
+        <v>23</v>
+      </c>
+      <c r="D14" s="13">
         <v>131</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>108</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="13">
         <v>148</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>137</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="13">
         <v>168</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>296</v>
       </c>
       <c r="J14" s="3">
@@ -1172,7 +1202,7 @@
       <c r="K14" s="3">
         <v>530</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="13">
         <v>1014</v>
       </c>
       <c r="M14" s="3">
@@ -1181,57 +1211,61 @@
       <c r="N14" s="3">
         <v>610</v>
       </c>
-      <c r="O14" s="3"/>
+      <c r="O14" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="A15" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="O15" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="14">
+        <v>29</v>
+      </c>
+      <c r="D16" s="13">
         <v>264</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>141</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <v>156</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>222</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <v>174</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <v>246</v>
       </c>
       <c r="J16" s="3">
@@ -1249,34 +1283,36 @@
       <c r="N16" s="3">
         <v>728</v>
       </c>
-      <c r="O16" s="3"/>
+      <c r="O16" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="14">
+        <v>30</v>
+      </c>
+      <c r="D17" s="13">
         <v>131</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>191</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>164</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>121</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="13">
         <v>87</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="13">
         <v>173</v>
       </c>
       <c r="J17" s="3">
@@ -1294,34 +1330,36 @@
       <c r="N17" s="3">
         <v>407</v>
       </c>
-      <c r="O17" s="3"/>
+      <c r="O17" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="14">
+        <v>37</v>
+      </c>
+      <c r="D18" s="13">
         <v>523</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>495</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <v>359</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>421</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <v>483</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <v>318</v>
       </c>
       <c r="J18" s="3">
@@ -1330,43 +1368,45 @@
       <c r="K18" s="3">
         <v>1226</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="13">
         <v>1035</v>
       </c>
-      <c r="M18" s="14">
+      <c r="M18" s="13">
         <v>1223</v>
       </c>
       <c r="N18" s="3">
         <v>1177</v>
       </c>
-      <c r="O18" s="3"/>
+      <c r="O18" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="14">
+        <v>38</v>
+      </c>
+      <c r="D19" s="13">
         <v>1101</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>795</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="13">
         <v>1072</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>1647</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="13">
         <v>1588</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="13">
         <v>1839</v>
       </c>
       <c r="J19" s="3">
@@ -1375,43 +1415,45 @@
       <c r="K19" s="3">
         <v>4436</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="13">
         <v>4793</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19" s="13">
         <v>4228</v>
       </c>
       <c r="N19" s="3">
         <v>3381</v>
       </c>
-      <c r="O19" s="3"/>
+      <c r="O19" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="14">
+        <v>31</v>
+      </c>
+      <c r="D20" s="13">
         <v>74</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <v>167</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="13">
         <v>58</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>4</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <v>7</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <v>42</v>
       </c>
       <c r="J20" s="3">
@@ -1429,57 +1471,61 @@
       <c r="N20" s="3">
         <v>452</v>
       </c>
-      <c r="O20" s="3"/>
+      <c r="O20" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
+      <c r="A21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="O21" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="14">
+        <v>33</v>
+      </c>
+      <c r="D22" s="13">
         <v>533</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="13">
         <v>560</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="13">
         <v>493</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>478</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="13">
         <v>383</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="13">
         <v>464</v>
       </c>
       <c r="J22" s="3">
@@ -1488,43 +1534,45 @@
       <c r="K22" s="3">
         <v>1658</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="13">
         <v>1516</v>
       </c>
-      <c r="M22" s="14">
+      <c r="M22" s="13">
         <v>1818</v>
       </c>
       <c r="N22" s="3">
         <v>1178</v>
       </c>
-      <c r="O22" s="3"/>
+      <c r="O22" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="14">
+        <v>35</v>
+      </c>
+      <c r="D23" s="13">
         <v>1384</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="13">
         <v>1106</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="13">
         <v>1232</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <v>1814</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H23" s="13">
         <v>1810</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="13">
         <v>1916</v>
       </c>
       <c r="J23" s="3">
@@ -1533,43 +1581,45 @@
       <c r="K23" s="3">
         <v>4906</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="13">
         <v>5164</v>
       </c>
-      <c r="M23" s="14">
+      <c r="M23" s="13">
         <v>4681</v>
       </c>
       <c r="N23" s="3">
         <v>4290</v>
       </c>
-      <c r="O23" s="3"/>
+      <c r="O23" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="14">
+        <v>34</v>
+      </c>
+      <c r="D24" s="13">
         <v>82</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <v>30</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="13">
         <v>14</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>36</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="13">
         <v>61</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="13">
         <v>95</v>
       </c>
       <c r="J24" s="3">
@@ -1587,34 +1637,36 @@
       <c r="N24" s="3">
         <v>318</v>
       </c>
-      <c r="O24" s="3"/>
+      <c r="O24" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="15">
+        <v>36</v>
+      </c>
+      <c r="D25" s="14">
         <v>94</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>93</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="14">
         <v>70</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="14">
         <v>87</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>85</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="14">
         <v>143</v>
       </c>
       <c r="J25" s="5">
@@ -1632,7 +1684,9 @@
       <c r="N25" s="5">
         <v>359</v>
       </c>
-      <c r="O25" s="3"/>
+      <c r="O25" s="20" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1653,5 +1707,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>